<commit_message>
update finding bearings algorithm
</commit_message>
<xml_diff>
--- a/data/Data Temperature Dummy.xlsx
+++ b/data/Data Temperature Dummy.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nur Jamiludin\Documents\GitHub\bearing_temperature_monitoring_app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khout\OneDrive\Documents\Github\bearing_temperature_monitoring_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6594CFCD-5C83-425D-9217-590D3CC29609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,20 +346,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AV15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="101" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="101" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,7 +367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -448,7 +447,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -528,7 +527,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -608,7 +607,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -688,7 +687,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -768,7 +767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -848,7 +847,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -928,7 +927,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1008,7 +1007,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1088,7 +1087,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1168,7 +1167,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1248,7 +1247,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1328,7 +1327,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1406,6 +1405,77 @@
       </c>
       <c r="Z14">
         <v>82</v>
+      </c>
+      <c r="AA14">
+        <v>81.906999999999996</v>
+      </c>
+      <c r="AB14">
+        <v>81.922615384615398</v>
+      </c>
+      <c r="AC14">
+        <v>81.938230769230799</v>
+      </c>
+      <c r="AD14">
+        <v>81.9538461538462</v>
+      </c>
+      <c r="AE14">
+        <v>81.969461538461502</v>
+      </c>
+      <c r="AF14">
+        <v>81.985076923076903</v>
+      </c>
+      <c r="AG14">
+        <v>82.000692307692304</v>
+      </c>
+      <c r="AH14">
+        <v>82.016307692307706</v>
+      </c>
+      <c r="AI14">
+        <v>82.031923076923107</v>
+      </c>
+      <c r="AJ14">
+        <v>82.047538461538494</v>
+      </c>
+      <c r="AK14">
+        <v>82.063153846153895</v>
+      </c>
+      <c r="AL14">
+        <v>82.078769230769197</v>
+      </c>
+      <c r="AM14">
+        <v>82.094384615384598</v>
+      </c>
+      <c r="AN14">
+        <v>82.11</v>
+      </c>
+      <c r="AO14">
+        <v>82.125615384615401</v>
+      </c>
+      <c r="AP14">
+        <v>82.141230769230802</v>
+      </c>
+      <c r="AQ14">
+        <v>82.156846153846203</v>
+      </c>
+      <c r="AR14">
+        <v>82.172461538461505</v>
+      </c>
+      <c r="AS14">
+        <v>82.188076923076906</v>
+      </c>
+      <c r="AT14">
+        <v>82.203692307692293</v>
+      </c>
+      <c r="AU14">
+        <v>82.219307692307694</v>
+      </c>
+      <c r="AV14">
+        <v>82.234923076923096</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>